<commit_message>
datamaps & data - converter
</commit_message>
<xml_diff>
--- a/[Data] GenderGap/GenderGap_Find4Hourglass.xlsx
+++ b/[Data] GenderGap/GenderGap_Find4Hourglass.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="5320" windowWidth="22500" windowHeight="13620" tabRatio="624" activeTab="9"/>
+    <workbookView xWindow="700" yWindow="0" windowWidth="35940" windowHeight="17780" tabRatio="624" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="13C_csv" sheetId="10" r:id="rId1"/>
@@ -1812,43 +1812,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="105" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1863,19 +1829,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1890,6 +1844,54 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="2" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="106" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="15" xfId="108" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="16" xfId="108" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1897,8 +1899,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="105" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="105" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="239">
     <cellStyle name="Bad" xfId="107" builtinId="27"/>
@@ -2514,11 +2514,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="2133376968"/>
-        <c:axId val="2133379992"/>
+        <c:axId val="2087799032"/>
+        <c:axId val="2087802008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2133376968"/>
+        <c:axId val="2087799032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2527,7 +2527,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133379992"/>
+        <c:crossAx val="2087802008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2535,7 +2535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133379992"/>
+        <c:axId val="2087802008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2551,7 +2551,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2133376968"/>
+        <c:crossAx val="2087799032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2766,11 +2766,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2133457464"/>
-        <c:axId val="2133460408"/>
+        <c:axId val="2087865752"/>
+        <c:axId val="2087868696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2133457464"/>
+        <c:axId val="2087865752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2779,7 +2779,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2133460408"/>
+        <c:crossAx val="2087868696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2787,7 +2787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2133460408"/>
+        <c:axId val="2087868696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2798,7 @@
         <c:majorTickMark val="in"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="2133457464"/>
+        <c:crossAx val="2087865752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3224,7 +3224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB50"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E31" sqref="E31:R31"/>
     </sheetView>
   </sheetViews>
@@ -6274,156 +6274,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" style="143" customWidth="1"/>
-    <col min="2" max="2" width="26" style="143" customWidth="1"/>
-    <col min="3" max="3" width="40.5" style="143" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="143" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="143"/>
+    <col min="1" max="1" width="49.33203125" style="114" customWidth="1"/>
+    <col min="2" max="2" width="26" style="114" customWidth="1"/>
+    <col min="3" max="3" width="40.5" style="114" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="114" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="114"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1">
-      <c r="A1" s="142" t="s">
+      <c r="A1" s="144" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142" t="s">
+      <c r="B1" s="144"/>
+      <c r="C1" s="144"/>
+      <c r="D1" s="144"/>
+      <c r="E1" s="144"/>
+      <c r="F1" s="144" t="s">
         <v>202</v>
       </c>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
-      <c r="J1" s="142" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="142"/>
-      <c r="L1" s="142" t="s">
+      <c r="G1" s="144"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="144"/>
+      <c r="J1" s="144" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="144"/>
+      <c r="L1" s="144" t="s">
         <v>203</v>
       </c>
-      <c r="M1" s="142"/>
-      <c r="N1" s="142"/>
+      <c r="M1" s="144"/>
+      <c r="N1" s="144"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="143" t="s">
+      <c r="A2" s="114" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="143" t="s">
+      <c r="B2" s="114" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="143" t="s">
+      <c r="C2" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="143" t="s">
+      <c r="D2" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="143" t="s">
+      <c r="E2" s="114" t="s">
         <v>205</v>
       </c>
-      <c r="F2" s="143" t="s">
+      <c r="F2" s="114" t="s">
         <v>206</v>
       </c>
-      <c r="G2" s="143" t="s">
+      <c r="G2" s="114" t="s">
         <v>207</v>
       </c>
-      <c r="H2" s="143" t="s">
+      <c r="H2" s="114" t="s">
         <v>208</v>
       </c>
-      <c r="I2" s="143" t="s">
+      <c r="I2" s="114" t="s">
         <v>209</v>
       </c>
-      <c r="J2" s="143" t="s">
+      <c r="J2" s="114" t="s">
         <v>210</v>
       </c>
-      <c r="K2" s="143" t="s">
+      <c r="K2" s="114" t="s">
         <v>211</v>
       </c>
-      <c r="L2" s="143" t="s">
+      <c r="L2" s="114" t="s">
         <v>212</v>
       </c>
-      <c r="M2" s="143" t="s">
+      <c r="M2" s="114" t="s">
         <v>213</v>
       </c>
-      <c r="N2" s="143" t="s">
+      <c r="N2" s="114" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="142" t="s">
+      <c r="A3" s="144" t="s">
         <v>201</v>
       </c>
-      <c r="B3" s="142"/>
-      <c r="C3" s="142"/>
-      <c r="D3" s="142"/>
-      <c r="E3" s="142"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="143" t="s">
+      <c r="A7" s="114" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="114" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="143" t="s">
+      <c r="C7" s="114" t="s">
         <v>197</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="114" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="143" t="s">
+      <c r="A8" s="114" t="s">
         <v>200</v>
       </c>
       <c r="B8" s="26">
         <v>0.84</v>
       </c>
-      <c r="C8" s="143" t="s">
+      <c r="C8" s="114" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="143" t="s">
+      <c r="A9" s="114" t="s">
         <v>204</v>
       </c>
       <c r="B9" s="26">
         <v>0.63</v>
       </c>
-      <c r="C9" s="144" t="s">
+      <c r="C9" s="115" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="143" t="s">
+      <c r="A10" s="114" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="26">
         <v>0.64</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="114" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="143" t="s">
+      <c r="A11" s="114" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="26">
         <v>0.2</v>
       </c>
-      <c r="C11" s="143" t="s">
+      <c r="C11" s="114" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="143" t="s">
+      <c r="A12" s="114" t="s">
         <v>205</v>
       </c>
       <c r="B12" s="26">
@@ -6431,7 +6431,7 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="143" t="s">
+      <c r="A13" s="114" t="s">
         <v>206</v>
       </c>
       <c r="B13" s="34">
@@ -6439,7 +6439,7 @@
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="143" t="s">
+      <c r="A14" s="114" t="s">
         <v>218</v>
       </c>
       <c r="B14" s="34">
@@ -6447,7 +6447,7 @@
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="143" t="s">
+      <c r="A15" s="114" t="s">
         <v>219</v>
       </c>
       <c r="B15" s="34" t="s">
@@ -6455,7 +6455,7 @@
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="143" t="s">
+      <c r="A16" s="114" t="s">
         <v>220</v>
       </c>
       <c r="B16" s="34">
@@ -6463,7 +6463,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="143" t="s">
+      <c r="A17" s="114" t="s">
         <v>210</v>
       </c>
       <c r="B17" s="28">
@@ -6471,7 +6471,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="143" t="s">
+      <c r="A18" s="114" t="s">
         <v>211</v>
       </c>
       <c r="B18" s="28">
@@ -6479,7 +6479,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="143" t="s">
+      <c r="A19" s="114" t="s">
         <v>212</v>
       </c>
       <c r="B19" s="34">
@@ -6487,7 +6487,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="143" t="s">
+      <c r="A20" s="114" t="s">
         <v>213</v>
       </c>
       <c r="B20" s="34">
@@ -6495,7 +6495,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="143" t="s">
+      <c r="A21" s="114" t="s">
         <v>214</v>
       </c>
       <c r="B21" s="34">
@@ -6524,8 +6524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W2" sqref="T1:W2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6554,37 +6554,37 @@
     <row r="1" spans="1:27" ht="34" customHeight="1">
       <c r="A1" s="97"/>
       <c r="B1" s="97"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -6601,9 +6601,9 @@
     <row r="2" spans="1:27" ht="113" customHeight="1">
       <c r="A2" s="97"/>
       <c r="B2" s="97"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -6672,13 +6672,13 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="127">
-        <v>1</v>
-      </c>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="117">
+        <v>1</v>
+      </c>
+      <c r="C3" s="120" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="92">
@@ -6746,9 +6746,9 @@
       </c>
     </row>
     <row r="4" spans="1:27">
-      <c r="A4" s="137"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="92">
         <v>2010</v>
       </c>
@@ -6814,9 +6814,9 @@
       </c>
     </row>
     <row r="5" spans="1:27">
-      <c r="A5" s="137"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="123"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="120"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -6882,7 +6882,7 @@
       </c>
     </row>
     <row r="6" spans="1:27">
-      <c r="A6" s="137"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="91"/>
       <c r="C6" s="92"/>
       <c r="D6" s="25"/>
@@ -6904,11 +6904,11 @@
       <c r="X6" s="106"/>
     </row>
     <row r="7" spans="1:27" ht="15" customHeight="1">
-      <c r="A7" s="137"/>
-      <c r="B7" s="127">
+      <c r="A7" s="123"/>
+      <c r="B7" s="117">
         <v>2</v>
       </c>
-      <c r="C7" s="130" t="s">
+      <c r="C7" s="120" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="92">
@@ -6976,9 +6976,9 @@
       </c>
     </row>
     <row r="8" spans="1:27">
-      <c r="A8" s="137"/>
-      <c r="B8" s="128"/>
-      <c r="C8" s="130"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="120"/>
       <c r="D8" s="92">
         <v>2010</v>
       </c>
@@ -7044,9 +7044,9 @@
       </c>
     </row>
     <row r="9" spans="1:27">
-      <c r="A9" s="137"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="130"/>
+      <c r="A9" s="123"/>
+      <c r="B9" s="119"/>
+      <c r="C9" s="120"/>
       <c r="D9" s="25">
         <v>2014</v>
       </c>
@@ -7112,7 +7112,7 @@
       </c>
     </row>
     <row r="10" spans="1:27">
-      <c r="A10" s="137"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="91"/>
       <c r="C10" s="92"/>
       <c r="D10" s="25"/>
@@ -7134,11 +7134,11 @@
       <c r="X10" s="106"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A11" s="137"/>
-      <c r="B11" s="127">
+      <c r="A11" s="123"/>
+      <c r="B11" s="117">
         <v>3</v>
       </c>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="120" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="92">
@@ -7206,9 +7206,9 @@
       </c>
     </row>
     <row r="12" spans="1:27">
-      <c r="A12" s="137"/>
-      <c r="B12" s="128"/>
-      <c r="C12" s="130"/>
+      <c r="A12" s="123"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="120"/>
       <c r="D12" s="92">
         <v>2010</v>
       </c>
@@ -7274,9 +7274,9 @@
       </c>
     </row>
     <row r="13" spans="1:27">
-      <c r="A13" s="137"/>
-      <c r="B13" s="129"/>
-      <c r="C13" s="130"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="119"/>
+      <c r="C13" s="120"/>
       <c r="D13" s="25">
         <v>2014</v>
       </c>
@@ -7342,7 +7342,7 @@
       </c>
     </row>
     <row r="14" spans="1:27">
-      <c r="A14" s="137"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="91"/>
       <c r="C14" s="92"/>
       <c r="D14" s="25"/>
@@ -7364,11 +7364,11 @@
       <c r="X14" s="106"/>
     </row>
     <row r="15" spans="1:27">
-      <c r="A15" s="137"/>
-      <c r="B15" s="127">
+      <c r="A15" s="123"/>
+      <c r="B15" s="117">
         <v>4</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="120" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="92">
@@ -7436,9 +7436,9 @@
       </c>
     </row>
     <row r="16" spans="1:27">
-      <c r="A16" s="137"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="123"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="120"/>
       <c r="D16" s="92">
         <v>2010</v>
       </c>
@@ -7504,9 +7504,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="137"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="130"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="120"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -7572,7 +7572,7 @@
       </c>
     </row>
     <row r="18" spans="1:24">
-      <c r="A18" s="137"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="91"/>
       <c r="C18" s="92"/>
       <c r="D18" s="25"/>
@@ -7594,11 +7594,11 @@
       <c r="X18" s="106"/>
     </row>
     <row r="19" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A19" s="137"/>
-      <c r="B19" s="127">
+      <c r="A19" s="123"/>
+      <c r="B19" s="117">
         <v>5</v>
       </c>
-      <c r="C19" s="130" t="s">
+      <c r="C19" s="120" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="92">
@@ -7666,9 +7666,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="137"/>
-      <c r="B20" s="128"/>
-      <c r="C20" s="130"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="92">
         <v>2010</v>
       </c>
@@ -7734,9 +7734,9 @@
       </c>
     </row>
     <row r="21" spans="1:24">
-      <c r="A21" s="137"/>
-      <c r="B21" s="129"/>
-      <c r="C21" s="130"/>
+      <c r="A21" s="123"/>
+      <c r="B21" s="119"/>
+      <c r="C21" s="120"/>
       <c r="D21" s="25">
         <v>2014</v>
       </c>
@@ -7802,7 +7802,7 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="137"/>
+      <c r="A22" s="123"/>
       <c r="B22" s="91"/>
       <c r="C22" s="92"/>
       <c r="D22" s="25"/>
@@ -7824,11 +7824,11 @@
       <c r="X22" s="106"/>
     </row>
     <row r="23" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A23" s="137"/>
-      <c r="B23" s="127">
+      <c r="A23" s="123"/>
+      <c r="B23" s="117">
         <v>6</v>
       </c>
-      <c r="C23" s="130" t="s">
+      <c r="C23" s="120" t="s">
         <v>25</v>
       </c>
       <c r="D23" s="92">
@@ -7896,9 +7896,9 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="137"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="130"/>
+      <c r="A24" s="123"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="120"/>
       <c r="D24" s="92">
         <v>2010</v>
       </c>
@@ -7964,9 +7964,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="137"/>
-      <c r="B25" s="129"/>
-      <c r="C25" s="130"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="120"/>
       <c r="D25" s="25">
         <v>2014</v>
       </c>
@@ -8032,7 +8032,7 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="137"/>
+      <c r="A26" s="123"/>
       <c r="B26" s="91"/>
       <c r="C26" s="92"/>
       <c r="D26" s="25"/>
@@ -8054,11 +8054,11 @@
       <c r="X26" s="106"/>
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A27" s="137"/>
-      <c r="B27" s="127">
+      <c r="A27" s="123"/>
+      <c r="B27" s="117">
         <v>7</v>
       </c>
-      <c r="C27" s="130" t="s">
+      <c r="C27" s="120" t="s">
         <v>70</v>
       </c>
       <c r="D27" s="92">
@@ -8126,9 +8126,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="137"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="130"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="120"/>
       <c r="D28" s="92">
         <v>2010</v>
       </c>
@@ -8194,9 +8194,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="137"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="130"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="120"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -8262,7 +8262,7 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="137"/>
+      <c r="A30" s="123"/>
       <c r="B30" s="91"/>
       <c r="C30" s="95"/>
       <c r="D30" s="25"/>
@@ -8284,11 +8284,11 @@
       <c r="X30" s="106"/>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="137"/>
-      <c r="B31" s="127">
+      <c r="A31" s="123"/>
+      <c r="B31" s="117">
         <v>8</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" s="126" t="s">
         <v>54</v>
       </c>
       <c r="D31" s="92">
@@ -8356,9 +8356,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="137"/>
-      <c r="B32" s="128"/>
-      <c r="C32" s="132"/>
+      <c r="A32" s="123"/>
+      <c r="B32" s="118"/>
+      <c r="C32" s="127"/>
       <c r="D32" s="92">
         <v>2010</v>
       </c>
@@ -8424,9 +8424,9 @@
       </c>
     </row>
     <row r="33" spans="1:24">
-      <c r="A33" s="137"/>
-      <c r="B33" s="129"/>
-      <c r="C33" s="133"/>
+      <c r="A33" s="123"/>
+      <c r="B33" s="119"/>
+      <c r="C33" s="128"/>
       <c r="D33" s="25">
         <v>2014</v>
       </c>
@@ -8492,7 +8492,7 @@
       </c>
     </row>
     <row r="34" spans="1:24">
-      <c r="A34" s="137"/>
+      <c r="A34" s="123"/>
       <c r="B34" s="91"/>
       <c r="C34" s="96"/>
       <c r="D34" s="25"/>
@@ -8514,11 +8514,11 @@
       <c r="X34" s="106"/>
     </row>
     <row r="35" spans="1:24">
-      <c r="A35" s="137"/>
-      <c r="B35" s="127">
+      <c r="A35" s="123"/>
+      <c r="B35" s="117">
         <v>9</v>
       </c>
-      <c r="C35" s="130" t="s">
+      <c r="C35" s="120" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="92">
@@ -8586,9 +8586,9 @@
       </c>
     </row>
     <row r="36" spans="1:24">
-      <c r="A36" s="137"/>
-      <c r="B36" s="128"/>
-      <c r="C36" s="130"/>
+      <c r="A36" s="123"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="120"/>
       <c r="D36" s="92">
         <v>2010</v>
       </c>
@@ -8654,9 +8654,9 @@
       </c>
     </row>
     <row r="37" spans="1:24">
-      <c r="A37" s="137"/>
-      <c r="B37" s="129"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="123"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="120"/>
       <c r="D37" s="25">
         <v>2014</v>
       </c>
@@ -8722,7 +8722,7 @@
       </c>
     </row>
     <row r="38" spans="1:24">
-      <c r="A38" s="137"/>
+      <c r="A38" s="123"/>
       <c r="B38" s="91"/>
       <c r="C38" s="92"/>
       <c r="D38" s="25"/>
@@ -8744,11 +8744,11 @@
       <c r="X38" s="106"/>
     </row>
     <row r="39" spans="1:24">
-      <c r="A39" s="137"/>
-      <c r="B39" s="127">
+      <c r="A39" s="123"/>
+      <c r="B39" s="117">
         <v>10</v>
       </c>
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="120" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="92">
@@ -8816,9 +8816,9 @@
       </c>
     </row>
     <row r="40" spans="1:24">
-      <c r="A40" s="137"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="123"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="120"/>
       <c r="D40" s="92">
         <v>2010</v>
       </c>
@@ -8884,9 +8884,9 @@
       </c>
     </row>
     <row r="41" spans="1:24">
-      <c r="A41" s="137"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="130"/>
+      <c r="A41" s="123"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="120"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -8952,7 +8952,7 @@
       </c>
     </row>
     <row r="42" spans="1:24">
-      <c r="A42" s="137"/>
+      <c r="A42" s="123"/>
       <c r="B42" s="91"/>
       <c r="C42" s="92"/>
       <c r="D42" s="25"/>
@@ -8974,11 +8974,11 @@
       <c r="X42" s="106"/>
     </row>
     <row r="43" spans="1:24">
-      <c r="A43" s="137"/>
-      <c r="B43" s="127">
+      <c r="A43" s="123"/>
+      <c r="B43" s="117">
         <v>11</v>
       </c>
-      <c r="C43" s="130" t="s">
+      <c r="C43" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="92">
@@ -9046,9 +9046,9 @@
       </c>
     </row>
     <row r="44" spans="1:24">
-      <c r="A44" s="137"/>
-      <c r="B44" s="128"/>
-      <c r="C44" s="130"/>
+      <c r="A44" s="123"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="120"/>
       <c r="D44" s="92">
         <v>2010</v>
       </c>
@@ -9114,9 +9114,9 @@
       </c>
     </row>
     <row r="45" spans="1:24">
-      <c r="A45" s="137"/>
-      <c r="B45" s="129"/>
-      <c r="C45" s="130"/>
+      <c r="A45" s="123"/>
+      <c r="B45" s="119"/>
+      <c r="C45" s="120"/>
       <c r="D45" s="25">
         <v>2014</v>
       </c>
@@ -9182,7 +9182,7 @@
       </c>
     </row>
     <row r="46" spans="1:24">
-      <c r="A46" s="137"/>
+      <c r="A46" s="123"/>
       <c r="B46" s="91"/>
       <c r="C46" s="92"/>
       <c r="D46" s="25"/>
@@ -9204,11 +9204,11 @@
       <c r="X46" s="106"/>
     </row>
     <row r="47" spans="1:24">
-      <c r="A47" s="137"/>
-      <c r="B47" s="127">
+      <c r="A47" s="123"/>
+      <c r="B47" s="117">
         <v>12</v>
       </c>
-      <c r="C47" s="130" t="s">
+      <c r="C47" s="120" t="s">
         <v>13</v>
       </c>
       <c r="D47" s="92">
@@ -9276,9 +9276,9 @@
       </c>
     </row>
     <row r="48" spans="1:24">
-      <c r="A48" s="137"/>
-      <c r="B48" s="128"/>
-      <c r="C48" s="130"/>
+      <c r="A48" s="123"/>
+      <c r="B48" s="118"/>
+      <c r="C48" s="120"/>
       <c r="D48" s="92">
         <v>2010</v>
       </c>
@@ -9344,9 +9344,9 @@
       </c>
     </row>
     <row r="49" spans="1:41">
-      <c r="A49" s="137"/>
-      <c r="B49" s="129"/>
-      <c r="C49" s="130"/>
+      <c r="A49" s="123"/>
+      <c r="B49" s="119"/>
+      <c r="C49" s="120"/>
       <c r="D49" s="25">
         <v>2014</v>
       </c>
@@ -9412,7 +9412,7 @@
       </c>
     </row>
     <row r="50" spans="1:41">
-      <c r="A50" s="137"/>
+      <c r="A50" s="123"/>
       <c r="B50" s="91"/>
       <c r="C50" s="92"/>
       <c r="D50" s="25"/>
@@ -9434,11 +9434,11 @@
       <c r="X50" s="106"/>
     </row>
     <row r="51" spans="1:41">
-      <c r="A51" s="137"/>
-      <c r="B51" s="127">
+      <c r="A51" s="123"/>
+      <c r="B51" s="117">
         <v>13</v>
       </c>
-      <c r="C51" s="130" t="s">
+      <c r="C51" s="120" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="92">
@@ -9506,9 +9506,9 @@
       </c>
     </row>
     <row r="52" spans="1:41">
-      <c r="A52" s="137"/>
-      <c r="B52" s="128"/>
-      <c r="C52" s="130"/>
+      <c r="A52" s="123"/>
+      <c r="B52" s="118"/>
+      <c r="C52" s="120"/>
       <c r="D52" s="92">
         <v>2010</v>
       </c>
@@ -9574,9 +9574,9 @@
       </c>
     </row>
     <row r="53" spans="1:41">
-      <c r="A53" s="137"/>
-      <c r="B53" s="129"/>
-      <c r="C53" s="130"/>
+      <c r="A53" s="123"/>
+      <c r="B53" s="119"/>
+      <c r="C53" s="120"/>
       <c r="D53" s="25">
         <v>2014</v>
       </c>
@@ -9642,79 +9642,79 @@
       </c>
     </row>
     <row r="54" spans="1:41">
-      <c r="A54" s="137"/>
+      <c r="A54" s="123"/>
     </row>
     <row r="55" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A55" s="137"/>
+      <c r="A55" s="123"/>
       <c r="B55" s="86"/>
-      <c r="C55" s="114" t="s">
+      <c r="C55" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="114"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="114" t="s">
+      <c r="D55" s="132"/>
+      <c r="E55" s="132"/>
+      <c r="F55" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="G55" s="114"/>
-      <c r="H55" s="114"/>
-      <c r="I55" s="114" t="s">
+      <c r="G55" s="132"/>
+      <c r="H55" s="132"/>
+      <c r="I55" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="J55" s="114"/>
-      <c r="K55" s="114"/>
-      <c r="L55" s="114" t="s">
+      <c r="J55" s="132"/>
+      <c r="K55" s="132"/>
+      <c r="L55" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="M55" s="114"/>
-      <c r="N55" s="114"/>
-      <c r="O55" s="114" t="s">
+      <c r="M55" s="132"/>
+      <c r="N55" s="132"/>
+      <c r="O55" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="P55" s="114"/>
-      <c r="Q55" s="114"/>
-      <c r="R55" s="122" t="s">
+      <c r="P55" s="132"/>
+      <c r="Q55" s="132"/>
+      <c r="R55" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="123"/>
-      <c r="T55" s="124"/>
-      <c r="U55" s="114" t="s">
+      <c r="S55" s="130"/>
+      <c r="T55" s="131"/>
+      <c r="U55" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="V55" s="114"/>
-      <c r="W55" s="114"/>
-      <c r="X55" s="122" t="s">
+      <c r="V55" s="132"/>
+      <c r="W55" s="132"/>
+      <c r="X55" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="Y55" s="123"/>
-      <c r="Z55" s="124"/>
-      <c r="AA55" s="114" t="s">
+      <c r="Y55" s="130"/>
+      <c r="Z55" s="131"/>
+      <c r="AA55" s="132" t="s">
         <v>105</v>
       </c>
-      <c r="AB55" s="114"/>
-      <c r="AC55" s="114"/>
-      <c r="AD55" s="114" t="s">
+      <c r="AB55" s="132"/>
+      <c r="AC55" s="132"/>
+      <c r="AD55" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="114"/>
-      <c r="AF55" s="114"/>
-      <c r="AG55" s="114" t="s">
+      <c r="AE55" s="132"/>
+      <c r="AF55" s="132"/>
+      <c r="AG55" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="AH55" s="114"/>
-      <c r="AI55" s="114"/>
-      <c r="AJ55" s="114" t="s">
+      <c r="AH55" s="132"/>
+      <c r="AI55" s="132"/>
+      <c r="AJ55" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="114"/>
-      <c r="AL55" s="114"/>
-      <c r="AM55" s="114" t="s">
+      <c r="AK55" s="132"/>
+      <c r="AL55" s="132"/>
+      <c r="AM55" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="AN55" s="114"/>
-      <c r="AO55" s="114"/>
+      <c r="AN55" s="132"/>
+      <c r="AO55" s="132"/>
     </row>
     <row r="56" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A56" s="138"/>
+      <c r="A56" s="124"/>
       <c r="B56" s="86"/>
       <c r="C56" s="86" t="s">
         <v>72</v>
@@ -9955,10 +9955,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A58" s="125" t="s">
+      <c r="A58" s="133" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="126"/>
+      <c r="B58" s="134"/>
       <c r="C58" s="79">
         <v>2006</v>
       </c>
@@ -9995,10 +9995,10 @@
       <c r="Y58" s="105"/>
     </row>
     <row r="59" spans="1:41" ht="16" thickTop="1">
-      <c r="A59" s="119" t="s">
+      <c r="A59" s="135" t="s">
         <v>125</v>
       </c>
-      <c r="B59" s="119"/>
+      <c r="B59" s="135"/>
       <c r="C59">
         <f xml:space="preserve"> C57/115</f>
         <v>3.4782608695652174E-2</v>
@@ -10157,10 +10157,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="120" t="s">
+      <c r="A60" s="136" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="120"/>
+      <c r="B60" s="136"/>
       <c r="C60">
         <f xml:space="preserve"> C59*72</f>
         <v>2.5043478260869567</v>
@@ -10319,10 +10319,10 @@
       </c>
     </row>
     <row r="61" spans="1:41" s="80" customFormat="1">
-      <c r="A61" s="121" t="s">
+      <c r="A61" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="B61" s="121"/>
+      <c r="B61" s="137"/>
       <c r="C61" s="80">
         <f xml:space="preserve"> 72-C60</f>
         <v>69.495652173913044</v>
@@ -10632,77 +10632,77 @@
       <c r="X66" s="85"/>
     </row>
     <row r="67" spans="1:41">
-      <c r="C67" s="114" t="s">
+      <c r="C67" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="D67" s="114"/>
-      <c r="E67" s="114"/>
-      <c r="F67" s="122" t="s">
+      <c r="D67" s="132"/>
+      <c r="E67" s="132"/>
+      <c r="F67" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="G67" s="123"/>
-      <c r="H67" s="124"/>
-      <c r="I67" s="114" t="s">
+      <c r="G67" s="130"/>
+      <c r="H67" s="131"/>
+      <c r="I67" s="132" t="s">
         <v>105</v>
       </c>
-      <c r="J67" s="114"/>
-      <c r="K67" s="114"/>
-      <c r="L67" s="114" t="s">
+      <c r="J67" s="132"/>
+      <c r="K67" s="132"/>
+      <c r="L67" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="M67" s="114"/>
-      <c r="N67" s="114"/>
-      <c r="O67" s="114" t="s">
+      <c r="M67" s="132"/>
+      <c r="N67" s="132"/>
+      <c r="O67" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="P67" s="114"/>
-      <c r="Q67" s="114"/>
-      <c r="R67" s="122" t="s">
+      <c r="P67" s="132"/>
+      <c r="Q67" s="132"/>
+      <c r="R67" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="S67" s="123"/>
-      <c r="T67" s="124"/>
-      <c r="U67" s="114" t="s">
+      <c r="S67" s="130"/>
+      <c r="T67" s="131"/>
+      <c r="U67" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="V67" s="114"/>
-      <c r="W67" s="114"/>
-      <c r="X67" s="114" t="s">
+      <c r="V67" s="132"/>
+      <c r="W67" s="132"/>
+      <c r="X67" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="Y67" s="114"/>
-      <c r="Z67" s="114"/>
-      <c r="AA67" s="114" t="s">
+      <c r="Y67" s="132"/>
+      <c r="Z67" s="132"/>
+      <c r="AA67" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="AB67" s="114"/>
-      <c r="AC67" s="114"/>
-      <c r="AD67" s="114" t="s">
+      <c r="AB67" s="132"/>
+      <c r="AC67" s="132"/>
+      <c r="AD67" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="AE67" s="114"/>
-      <c r="AF67" s="114"/>
-      <c r="AG67" s="114" t="s">
+      <c r="AE67" s="132"/>
+      <c r="AF67" s="132"/>
+      <c r="AG67" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="AH67" s="114"/>
-      <c r="AI67" s="114"/>
-      <c r="AJ67" s="114" t="s">
+      <c r="AH67" s="132"/>
+      <c r="AI67" s="132"/>
+      <c r="AJ67" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="AK67" s="114"/>
-      <c r="AL67" s="114"/>
-      <c r="AM67" s="114" t="s">
+      <c r="AK67" s="132"/>
+      <c r="AL67" s="132"/>
+      <c r="AM67" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="AN67" s="114"/>
-      <c r="AO67" s="114"/>
+      <c r="AN67" s="132"/>
+      <c r="AO67" s="132"/>
     </row>
     <row r="68" spans="1:41" ht="70">
-      <c r="A68" s="115" t="s">
+      <c r="A68" s="138" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="116"/>
+      <c r="B68" s="139"/>
       <c r="C68" s="86" t="s">
         <v>99</v>
       </c>
@@ -10822,8 +10822,8 @@
       </c>
     </row>
     <row r="69" spans="1:41" ht="16" thickBot="1">
-      <c r="A69" s="117"/>
-      <c r="B69" s="118"/>
+      <c r="A69" s="140"/>
+      <c r="B69" s="141"/>
       <c r="C69" s="86">
         <v>23</v>
       </c>
@@ -10943,10 +10943,10 @@
       </c>
     </row>
     <row r="70" spans="1:41" ht="16" thickTop="1">
-      <c r="A70" s="119" t="s">
+      <c r="A70" s="135" t="s">
         <v>125</v>
       </c>
-      <c r="B70" s="119"/>
+      <c r="B70" s="135"/>
       <c r="C70">
         <f xml:space="preserve"> C69/115</f>
         <v>0.2</v>
@@ -11105,10 +11105,10 @@
       </c>
     </row>
     <row r="71" spans="1:41">
-      <c r="A71" s="120" t="s">
+      <c r="A71" s="136" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="120"/>
+      <c r="B71" s="136"/>
       <c r="C71">
         <f xml:space="preserve"> C70*65</f>
         <v>13</v>
@@ -11267,10 +11267,10 @@
       </c>
     </row>
     <row r="72" spans="1:41">
-      <c r="A72" s="121" t="s">
+      <c r="A72" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="B72" s="121"/>
+      <c r="B72" s="137"/>
       <c r="C72" s="80">
         <f xml:space="preserve"> 65-C71</f>
         <v>52</v>
@@ -11435,6 +11435,58 @@
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="AJ67:AL67"/>
+    <mergeCell ref="AM67:AO67"/>
+    <mergeCell ref="A68:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="AD67:AF67"/>
+    <mergeCell ref="AG67:AI67"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="R67:T67"/>
+    <mergeCell ref="U67:W67"/>
+    <mergeCell ref="X67:Z67"/>
+    <mergeCell ref="AA67:AC67"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="I67:K67"/>
+    <mergeCell ref="L67:N67"/>
+    <mergeCell ref="O67:Q67"/>
+    <mergeCell ref="AM55:AO55"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="U55:W55"/>
+    <mergeCell ref="X55:Z55"/>
+    <mergeCell ref="AA55:AC55"/>
+    <mergeCell ref="AD55:AF55"/>
+    <mergeCell ref="AG55:AI55"/>
+    <mergeCell ref="AJ55:AL55"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="O55:Q55"/>
+    <mergeCell ref="R55:T55"/>
+    <mergeCell ref="B43:B45"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="C27:C29"/>
@@ -11451,58 +11503,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="R55:T55"/>
-    <mergeCell ref="B43:B45"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="AM55:AO55"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="U55:W55"/>
-    <mergeCell ref="X55:Z55"/>
-    <mergeCell ref="AA55:AC55"/>
-    <mergeCell ref="AD55:AF55"/>
-    <mergeCell ref="AG55:AI55"/>
-    <mergeCell ref="AJ55:AL55"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="O55:Q55"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="R67:T67"/>
-    <mergeCell ref="U67:W67"/>
-    <mergeCell ref="X67:Z67"/>
-    <mergeCell ref="AA67:AC67"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="I67:K67"/>
-    <mergeCell ref="L67:N67"/>
-    <mergeCell ref="O67:Q67"/>
-    <mergeCell ref="AJ67:AL67"/>
-    <mergeCell ref="AM67:AO67"/>
-    <mergeCell ref="A68:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="AD67:AF67"/>
-    <mergeCell ref="AG67:AI67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -11546,37 +11546,37 @@
     <row r="1" spans="1:24" ht="34" customHeight="1">
       <c r="A1" s="57"/>
       <c r="B1" s="57"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="125" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
       <c r="T1" s="71" t="s">
         <v>92</v>
       </c>
@@ -11589,16 +11589,16 @@
       <c r="W1" s="71" t="s">
         <v>133</v>
       </c>
-      <c r="X1" s="130" t="s">
+      <c r="X1" s="120" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="144">
       <c r="A2" s="57"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -11653,16 +11653,16 @@
       <c r="W2" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="X2" s="130"/>
+      <c r="X2" s="120"/>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="127">
-        <v>1</v>
-      </c>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="117">
+        <v>1</v>
+      </c>
+      <c r="C3" s="120" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="54">
@@ -11730,9 +11730,9 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" s="137"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="54">
         <v>2010</v>
       </c>
@@ -11798,9 +11798,9 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" s="137"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="123"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="120"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -11866,11 +11866,11 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1">
-      <c r="A6" s="137"/>
-      <c r="B6" s="127">
+      <c r="A6" s="123"/>
+      <c r="B6" s="117">
         <v>2</v>
       </c>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="120" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="54">
@@ -11938,9 +11938,9 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" s="137"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="130"/>
+      <c r="A7" s="123"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="120"/>
       <c r="D7" s="54">
         <v>2010</v>
       </c>
@@ -12006,9 +12006,9 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" s="137"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="130"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="120"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -12074,11 +12074,11 @@
       </c>
     </row>
     <row r="9" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A9" s="137"/>
-      <c r="B9" s="127">
+      <c r="A9" s="123"/>
+      <c r="B9" s="117">
         <v>3</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="120" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="54">
@@ -12146,9 +12146,9 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" s="137"/>
-      <c r="B10" s="128"/>
-      <c r="C10" s="130"/>
+      <c r="A10" s="123"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="120"/>
       <c r="D10" s="54">
         <v>2010</v>
       </c>
@@ -12214,9 +12214,9 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" s="137"/>
-      <c r="B11" s="129"/>
-      <c r="C11" s="130"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="120"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -12282,11 +12282,11 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" s="137"/>
-      <c r="B12" s="127">
+      <c r="A12" s="123"/>
+      <c r="B12" s="117">
         <v>4</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="120" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="54">
@@ -12354,9 +12354,9 @@
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" s="137"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="130"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="120"/>
       <c r="D13" s="54">
         <v>2010</v>
       </c>
@@ -12422,9 +12422,9 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" s="137"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="130"/>
+      <c r="A14" s="123"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="120"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -12490,11 +12490,11 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A15" s="137"/>
-      <c r="B15" s="127">
+      <c r="A15" s="123"/>
+      <c r="B15" s="117">
         <v>5</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="120" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="54">
@@ -12562,9 +12562,9 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" s="137"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="123"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="120"/>
       <c r="D16" s="54">
         <v>2010</v>
       </c>
@@ -12630,9 +12630,9 @@
       </c>
     </row>
     <row r="17" spans="1:24">
-      <c r="A17" s="137"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="130"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="120"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -12698,11 +12698,11 @@
       </c>
     </row>
     <row r="18" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A18" s="137"/>
-      <c r="B18" s="127">
+      <c r="A18" s="123"/>
+      <c r="B18" s="117">
         <v>6</v>
       </c>
-      <c r="C18" s="130" t="s">
+      <c r="C18" s="120" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="54">
@@ -12770,9 +12770,9 @@
       </c>
     </row>
     <row r="19" spans="1:24">
-      <c r="A19" s="137"/>
-      <c r="B19" s="128"/>
-      <c r="C19" s="130"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="120"/>
       <c r="D19" s="54">
         <v>2010</v>
       </c>
@@ -12838,9 +12838,9 @@
       </c>
     </row>
     <row r="20" spans="1:24">
-      <c r="A20" s="137"/>
-      <c r="B20" s="129"/>
-      <c r="C20" s="130"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -12906,11 +12906,11 @@
       </c>
     </row>
     <row r="21" spans="1:24" ht="15.75" customHeight="1">
-      <c r="A21" s="137"/>
-      <c r="B21" s="127">
+      <c r="A21" s="123"/>
+      <c r="B21" s="117">
         <v>7</v>
       </c>
-      <c r="C21" s="130" t="s">
+      <c r="C21" s="120" t="s">
         <v>70</v>
       </c>
       <c r="D21" s="54">
@@ -12978,9 +12978,9 @@
       </c>
     </row>
     <row r="22" spans="1:24">
-      <c r="A22" s="137"/>
-      <c r="B22" s="128"/>
-      <c r="C22" s="130"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="120"/>
       <c r="D22" s="54">
         <v>2010</v>
       </c>
@@ -13046,9 +13046,9 @@
       </c>
     </row>
     <row r="23" spans="1:24">
-      <c r="A23" s="137"/>
-      <c r="B23" s="129"/>
-      <c r="C23" s="130"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="120"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -13114,11 +13114,11 @@
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="A24" s="137"/>
-      <c r="B24" s="127">
+      <c r="A24" s="123"/>
+      <c r="B24" s="117">
         <v>8</v>
       </c>
-      <c r="C24" s="131" t="s">
+      <c r="C24" s="126" t="s">
         <v>54</v>
       </c>
       <c r="D24" s="54">
@@ -13186,9 +13186,9 @@
       </c>
     </row>
     <row r="25" spans="1:24">
-      <c r="A25" s="137"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="132"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="127"/>
       <c r="D25" s="54">
         <v>2010</v>
       </c>
@@ -13254,9 +13254,9 @@
       </c>
     </row>
     <row r="26" spans="1:24">
-      <c r="A26" s="137"/>
-      <c r="B26" s="129"/>
-      <c r="C26" s="133"/>
+      <c r="A26" s="123"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="128"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -13322,11 +13322,11 @@
       </c>
     </row>
     <row r="27" spans="1:24">
-      <c r="A27" s="137"/>
-      <c r="B27" s="127">
+      <c r="A27" s="123"/>
+      <c r="B27" s="117">
         <v>9</v>
       </c>
-      <c r="C27" s="130" t="s">
+      <c r="C27" s="120" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="54">
@@ -13394,9 +13394,9 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="A28" s="137"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="130"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="120"/>
       <c r="D28" s="54">
         <v>2010</v>
       </c>
@@ -13462,9 +13462,9 @@
       </c>
     </row>
     <row r="29" spans="1:24">
-      <c r="A29" s="137"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="130"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="120"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -13530,11 +13530,11 @@
       </c>
     </row>
     <row r="30" spans="1:24">
-      <c r="A30" s="137"/>
-      <c r="B30" s="127">
+      <c r="A30" s="123"/>
+      <c r="B30" s="117">
         <v>10</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C30" s="120" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="54">
@@ -13602,9 +13602,9 @@
       </c>
     </row>
     <row r="31" spans="1:24">
-      <c r="A31" s="137"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="130"/>
+      <c r="A31" s="123"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="120"/>
       <c r="D31" s="54">
         <v>2010</v>
       </c>
@@ -13670,9 +13670,9 @@
       </c>
     </row>
     <row r="32" spans="1:24">
-      <c r="A32" s="137"/>
-      <c r="B32" s="129"/>
-      <c r="C32" s="130"/>
+      <c r="A32" s="123"/>
+      <c r="B32" s="119"/>
+      <c r="C32" s="120"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -13738,11 +13738,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="137"/>
-      <c r="B33" s="127">
+      <c r="A33" s="123"/>
+      <c r="B33" s="117">
         <v>11</v>
       </c>
-      <c r="C33" s="130" t="s">
+      <c r="C33" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D33" s="54">
@@ -13810,9 +13810,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="137"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="130"/>
+      <c r="A34" s="123"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="120"/>
       <c r="D34" s="54">
         <v>2010</v>
       </c>
@@ -13878,9 +13878,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="137"/>
-      <c r="B35" s="129"/>
-      <c r="C35" s="130"/>
+      <c r="A35" s="123"/>
+      <c r="B35" s="119"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -13946,11 +13946,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="137"/>
-      <c r="B36" s="127">
+      <c r="A36" s="123"/>
+      <c r="B36" s="117">
         <v>12</v>
       </c>
-      <c r="C36" s="130" t="s">
+      <c r="C36" s="120" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="54">
@@ -14018,9 +14018,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="137"/>
-      <c r="B37" s="128"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="123"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="120"/>
       <c r="D37" s="54">
         <v>2010</v>
       </c>
@@ -14086,9 +14086,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="137"/>
-      <c r="B38" s="129"/>
-      <c r="C38" s="130"/>
+      <c r="A38" s="123"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="120"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -14154,11 +14154,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="137"/>
-      <c r="B39" s="127">
+      <c r="A39" s="123"/>
+      <c r="B39" s="117">
         <v>13</v>
       </c>
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="120" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="54">
@@ -14226,9 +14226,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="137"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="123"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="120"/>
       <c r="D40" s="54">
         <v>2010</v>
       </c>
@@ -14294,9 +14294,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="137"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="130"/>
+      <c r="A41" s="123"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="120"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -14362,79 +14362,79 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="137"/>
+      <c r="A42" s="123"/>
     </row>
     <row r="43" spans="1:41" s="75" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A43" s="137"/>
+      <c r="A43" s="123"/>
       <c r="B43" s="73"/>
-      <c r="C43" s="114" t="s">
+      <c r="C43" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="114"/>
-      <c r="E43" s="114"/>
-      <c r="F43" s="114" t="s">
+      <c r="D43" s="132"/>
+      <c r="E43" s="132"/>
+      <c r="F43" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="G43" s="114"/>
-      <c r="H43" s="114"/>
-      <c r="I43" s="114" t="s">
+      <c r="G43" s="132"/>
+      <c r="H43" s="132"/>
+      <c r="I43" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="J43" s="114"/>
-      <c r="K43" s="114"/>
-      <c r="L43" s="114" t="s">
+      <c r="J43" s="132"/>
+      <c r="K43" s="132"/>
+      <c r="L43" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="114"/>
-      <c r="N43" s="114"/>
-      <c r="O43" s="114" t="s">
+      <c r="M43" s="132"/>
+      <c r="N43" s="132"/>
+      <c r="O43" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="P43" s="114"/>
-      <c r="Q43" s="114"/>
-      <c r="R43" s="122" t="s">
+      <c r="P43" s="132"/>
+      <c r="Q43" s="132"/>
+      <c r="R43" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="S43" s="123"/>
-      <c r="T43" s="124"/>
-      <c r="U43" s="114" t="s">
+      <c r="S43" s="130"/>
+      <c r="T43" s="131"/>
+      <c r="U43" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="V43" s="114"/>
-      <c r="W43" s="114"/>
-      <c r="X43" s="122" t="s">
+      <c r="V43" s="132"/>
+      <c r="W43" s="132"/>
+      <c r="X43" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="Y43" s="123"/>
-      <c r="Z43" s="124"/>
-      <c r="AA43" s="114" t="s">
+      <c r="Y43" s="130"/>
+      <c r="Z43" s="131"/>
+      <c r="AA43" s="132" t="s">
         <v>105</v>
       </c>
-      <c r="AB43" s="114"/>
-      <c r="AC43" s="114"/>
-      <c r="AD43" s="114" t="s">
+      <c r="AB43" s="132"/>
+      <c r="AC43" s="132"/>
+      <c r="AD43" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="AE43" s="114"/>
-      <c r="AF43" s="114"/>
-      <c r="AG43" s="114" t="s">
+      <c r="AE43" s="132"/>
+      <c r="AF43" s="132"/>
+      <c r="AG43" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="AH43" s="114"/>
-      <c r="AI43" s="114"/>
-      <c r="AJ43" s="114" t="s">
+      <c r="AH43" s="132"/>
+      <c r="AI43" s="132"/>
+      <c r="AJ43" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="AK43" s="114"/>
-      <c r="AL43" s="114"/>
-      <c r="AM43" s="114" t="s">
+      <c r="AK43" s="132"/>
+      <c r="AL43" s="132"/>
+      <c r="AM43" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="AN43" s="114"/>
-      <c r="AO43" s="114"/>
+      <c r="AN43" s="132"/>
+      <c r="AO43" s="132"/>
     </row>
     <row r="44" spans="1:41" s="75" customFormat="1" ht="70">
-      <c r="A44" s="138"/>
+      <c r="A44" s="124"/>
       <c r="B44" s="73"/>
       <c r="C44" s="73" t="s">
         <v>72</v>
@@ -14675,10 +14675,10 @@
       </c>
     </row>
     <row r="46" spans="1:41" s="79" customFormat="1" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="125" t="s">
+      <c r="A46" s="133" t="s">
         <v>129</v>
       </c>
-      <c r="B46" s="126"/>
+      <c r="B46" s="134"/>
       <c r="C46" s="79">
         <v>2006</v>
       </c>
@@ -14715,10 +14715,10 @@
       <c r="Y46" s="105"/>
     </row>
     <row r="47" spans="1:41" ht="16" thickTop="1">
-      <c r="A47" s="119" t="s">
+      <c r="A47" s="135" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="119"/>
+      <c r="B47" s="135"/>
       <c r="C47">
         <f xml:space="preserve"> C45/115</f>
         <v>3.4782608695652174E-2</v>
@@ -14877,10 +14877,10 @@
       </c>
     </row>
     <row r="48" spans="1:41">
-      <c r="A48" s="120" t="s">
+      <c r="A48" s="136" t="s">
         <v>124</v>
       </c>
-      <c r="B48" s="120"/>
+      <c r="B48" s="136"/>
       <c r="C48">
         <f xml:space="preserve"> C47*72</f>
         <v>2.5043478260869567</v>
@@ -15039,10 +15039,10 @@
       </c>
     </row>
     <row r="49" spans="1:41" s="80" customFormat="1">
-      <c r="A49" s="121" t="s">
+      <c r="A49" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="121"/>
+      <c r="B49" s="137"/>
       <c r="C49" s="80">
         <f xml:space="preserve"> 72-C48</f>
         <v>69.495652173913044</v>
@@ -15352,77 +15352,77 @@
       <c r="X54" s="85"/>
     </row>
     <row r="55" spans="1:41">
-      <c r="C55" s="114" t="s">
+      <c r="C55" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="D55" s="114"/>
-      <c r="E55" s="114"/>
-      <c r="F55" s="122" t="s">
+      <c r="D55" s="132"/>
+      <c r="E55" s="132"/>
+      <c r="F55" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="123"/>
-      <c r="H55" s="124"/>
-      <c r="I55" s="114" t="s">
+      <c r="G55" s="130"/>
+      <c r="H55" s="131"/>
+      <c r="I55" s="132" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="114"/>
-      <c r="K55" s="114"/>
-      <c r="L55" s="114" t="s">
+      <c r="J55" s="132"/>
+      <c r="K55" s="132"/>
+      <c r="L55" s="132" t="s">
         <v>50</v>
       </c>
-      <c r="M55" s="114"/>
-      <c r="N55" s="114"/>
-      <c r="O55" s="114" t="s">
+      <c r="M55" s="132"/>
+      <c r="N55" s="132"/>
+      <c r="O55" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="P55" s="114"/>
-      <c r="Q55" s="114"/>
-      <c r="R55" s="122" t="s">
+      <c r="P55" s="132"/>
+      <c r="Q55" s="132"/>
+      <c r="R55" s="129" t="s">
         <v>87</v>
       </c>
-      <c r="S55" s="123"/>
-      <c r="T55" s="124"/>
-      <c r="U55" s="114" t="s">
+      <c r="S55" s="130"/>
+      <c r="T55" s="131"/>
+      <c r="U55" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="V55" s="114"/>
-      <c r="W55" s="114"/>
-      <c r="X55" s="114" t="s">
+      <c r="V55" s="132"/>
+      <c r="W55" s="132"/>
+      <c r="X55" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="Y55" s="114"/>
-      <c r="Z55" s="114"/>
-      <c r="AA55" s="114" t="s">
+      <c r="Y55" s="132"/>
+      <c r="Z55" s="132"/>
+      <c r="AA55" s="132" t="s">
         <v>8</v>
       </c>
-      <c r="AB55" s="114"/>
-      <c r="AC55" s="114"/>
-      <c r="AD55" s="114" t="s">
+      <c r="AB55" s="132"/>
+      <c r="AC55" s="132"/>
+      <c r="AD55" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="AE55" s="114"/>
-      <c r="AF55" s="114"/>
-      <c r="AG55" s="114" t="s">
+      <c r="AE55" s="132"/>
+      <c r="AF55" s="132"/>
+      <c r="AG55" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="AH55" s="114"/>
-      <c r="AI55" s="114"/>
-      <c r="AJ55" s="114" t="s">
+      <c r="AH55" s="132"/>
+      <c r="AI55" s="132"/>
+      <c r="AJ55" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="AK55" s="114"/>
-      <c r="AL55" s="114"/>
-      <c r="AM55" s="114" t="s">
+      <c r="AK55" s="132"/>
+      <c r="AL55" s="132"/>
+      <c r="AM55" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="AN55" s="114"/>
-      <c r="AO55" s="114"/>
+      <c r="AN55" s="132"/>
+      <c r="AO55" s="132"/>
     </row>
     <row r="56" spans="1:41" ht="70">
-      <c r="A56" s="115" t="s">
+      <c r="A56" s="138" t="s">
         <v>128</v>
       </c>
-      <c r="B56" s="116"/>
+      <c r="B56" s="139"/>
       <c r="C56" s="74" t="s">
         <v>99</v>
       </c>
@@ -15542,8 +15542,8 @@
       </c>
     </row>
     <row r="57" spans="1:41" ht="16" thickBot="1">
-      <c r="A57" s="117"/>
-      <c r="B57" s="118"/>
+      <c r="A57" s="140"/>
+      <c r="B57" s="141"/>
       <c r="C57" s="74">
         <v>23</v>
       </c>
@@ -15663,10 +15663,10 @@
       </c>
     </row>
     <row r="58" spans="1:41" ht="16" thickTop="1">
-      <c r="A58" s="119" t="s">
+      <c r="A58" s="135" t="s">
         <v>125</v>
       </c>
-      <c r="B58" s="119"/>
+      <c r="B58" s="135"/>
       <c r="C58">
         <f xml:space="preserve"> C57/115</f>
         <v>0.2</v>
@@ -15825,10 +15825,10 @@
       </c>
     </row>
     <row r="59" spans="1:41">
-      <c r="A59" s="120" t="s">
+      <c r="A59" s="136" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="120"/>
+      <c r="B59" s="136"/>
       <c r="C59">
         <f xml:space="preserve"> C58*65</f>
         <v>13</v>
@@ -15987,10 +15987,10 @@
       </c>
     </row>
     <row r="60" spans="1:41">
-      <c r="A60" s="121" t="s">
+      <c r="A60" s="137" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="121"/>
+      <c r="B60" s="137"/>
       <c r="C60" s="80">
         <f xml:space="preserve"> 65-C59</f>
         <v>52</v>
@@ -16155,42 +16155,22 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="AD43:AF43"/>
-    <mergeCell ref="AG43:AI43"/>
-    <mergeCell ref="AJ43:AL43"/>
-    <mergeCell ref="AM43:AO43"/>
-    <mergeCell ref="X43:Z43"/>
-    <mergeCell ref="AA43:AC43"/>
-    <mergeCell ref="X1:X2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="O43:Q43"/>
-    <mergeCell ref="U43:W43"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A56:B57"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="AG55:AI55"/>
+    <mergeCell ref="AJ55:AL55"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="O55:Q55"/>
+    <mergeCell ref="U55:W55"/>
+    <mergeCell ref="X55:Z55"/>
+    <mergeCell ref="AA55:AC55"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="R55:T55"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="AM55:AO55"/>
     <mergeCell ref="A58:B58"/>
@@ -16207,23 +16187,43 @@
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="AJ43:AL43"/>
+    <mergeCell ref="AM43:AO43"/>
+    <mergeCell ref="X43:Z43"/>
+    <mergeCell ref="AA43:AC43"/>
+    <mergeCell ref="X1:X2"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AD43:AF43"/>
+    <mergeCell ref="AG43:AI43"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="O43:Q43"/>
+    <mergeCell ref="U43:W43"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
     <mergeCell ref="B30:B32"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A56:B57"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="AG55:AI55"/>
-    <mergeCell ref="AJ55:AL55"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="O55:Q55"/>
-    <mergeCell ref="U55:W55"/>
-    <mergeCell ref="X55:Z55"/>
-    <mergeCell ref="AA55:AC55"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="R55:T55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -16253,44 +16253,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -16335,7 +16335,7 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="122" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -16394,7 +16394,7 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="137"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -16451,7 +16451,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="137"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -16508,7 +16508,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -16565,7 +16565,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A7" s="137"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -16622,7 +16622,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A8" s="137"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -16679,7 +16679,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A9" s="137"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -16736,7 +16736,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -16793,7 +16793,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -16850,7 +16850,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -16907,7 +16907,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -16964,7 +16964,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -17021,7 +17021,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -17783,44 +17783,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -17865,7 +17865,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="122" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -17924,7 +17924,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="137"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -17981,7 +17981,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A5" s="137"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -18038,7 +18038,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -18095,7 +18095,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A7" s="137"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -18152,7 +18152,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="137"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -18209,7 +18209,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="25.5" customHeight="1">
-      <c r="A9" s="137"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -18266,7 +18266,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -18323,7 +18323,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -18380,7 +18380,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -18437,7 +18437,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -18494,7 +18494,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -18551,7 +18551,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -19365,44 +19365,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -19447,7 +19447,7 @@
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="122" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="44" t="s">
@@ -19506,7 +19506,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="24">
-      <c r="A4" s="137"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="45" t="s">
         <v>55</v>
       </c>
@@ -19563,7 +19563,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="24">
-      <c r="A5" s="137"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="45" t="s">
         <v>57</v>
       </c>
@@ -19620,7 +19620,7 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="45" t="s">
         <v>58</v>
       </c>
@@ -19677,7 +19677,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="24">
-      <c r="A7" s="137"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="45" t="s">
         <v>59</v>
       </c>
@@ -19734,7 +19734,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="24">
-      <c r="A8" s="137"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="45" t="s">
         <v>60</v>
       </c>
@@ -19791,7 +19791,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="24">
-      <c r="A9" s="137"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="45" t="s">
         <v>61</v>
       </c>
@@ -19848,7 +19848,7 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="45" t="s">
         <v>62</v>
       </c>
@@ -19905,7 +19905,7 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="45" t="s">
         <v>56</v>
       </c>
@@ -19962,7 +19962,7 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="45" t="s">
         <v>63</v>
       </c>
@@ -20019,7 +20019,7 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="45" t="s">
         <v>64</v>
       </c>
@@ -20076,7 +20076,7 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="45" t="s">
         <v>65</v>
       </c>
@@ -20133,7 +20133,7 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="45" t="s">
         <v>66</v>
       </c>
@@ -20254,171 +20254,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="20" customHeight="1">
-      <c r="C1" s="140" t="s">
+      <c r="C1" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="140"/>
-      <c r="E1" s="140"/>
-      <c r="F1" s="140"/>
-      <c r="G1" s="140"/>
-      <c r="H1" s="140"/>
-      <c r="I1" s="140"/>
-      <c r="J1" s="140"/>
-      <c r="K1" s="140"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="142"/>
+      <c r="I1" s="142"/>
+      <c r="J1" s="142"/>
+      <c r="K1" s="142"/>
     </row>
     <row r="2" spans="1:44" ht="20" customHeight="1">
-      <c r="C2" s="127">
-        <v>1</v>
-      </c>
-      <c r="D2" s="128"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="127">
+      <c r="C2" s="117">
+        <v>1</v>
+      </c>
+      <c r="D2" s="118"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="117">
         <v>2</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="127">
+      <c r="G2" s="118"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="117">
         <v>3</v>
       </c>
-      <c r="J2" s="128"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="127">
+      <c r="J2" s="118"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="117">
         <v>4</v>
       </c>
-      <c r="M2" s="128"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="127">
+      <c r="M2" s="118"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="117">
         <v>5</v>
       </c>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="129"/>
-      <c r="R2" s="127">
+      <c r="P2" s="118"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="117">
         <v>6</v>
       </c>
-      <c r="S2" s="128"/>
-      <c r="T2" s="129"/>
-      <c r="U2" s="127">
+      <c r="S2" s="118"/>
+      <c r="T2" s="119"/>
+      <c r="U2" s="117">
         <v>7</v>
       </c>
-      <c r="V2" s="128"/>
-      <c r="W2" s="129"/>
-      <c r="X2" s="127">
+      <c r="V2" s="118"/>
+      <c r="W2" s="119"/>
+      <c r="X2" s="117">
         <v>8</v>
       </c>
-      <c r="Y2" s="128"/>
-      <c r="Z2" s="129"/>
-      <c r="AA2" s="127">
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="119"/>
+      <c r="AA2" s="117">
         <v>14</v>
       </c>
-      <c r="AB2" s="128"/>
-      <c r="AC2" s="129"/>
-      <c r="AD2" s="127">
+      <c r="AB2" s="118"/>
+      <c r="AC2" s="119"/>
+      <c r="AD2" s="117">
         <v>9</v>
       </c>
-      <c r="AE2" s="128"/>
-      <c r="AF2" s="129"/>
-      <c r="AG2" s="127">
+      <c r="AE2" s="118"/>
+      <c r="AF2" s="119"/>
+      <c r="AG2" s="117">
         <v>10</v>
       </c>
-      <c r="AH2" s="128"/>
-      <c r="AI2" s="129"/>
-      <c r="AJ2" s="127">
+      <c r="AH2" s="118"/>
+      <c r="AI2" s="119"/>
+      <c r="AJ2" s="117">
         <v>11</v>
       </c>
-      <c r="AK2" s="128"/>
-      <c r="AL2" s="129"/>
-      <c r="AM2" s="127">
+      <c r="AK2" s="118"/>
+      <c r="AL2" s="119"/>
+      <c r="AM2" s="117">
         <v>12</v>
       </c>
-      <c r="AN2" s="128"/>
-      <c r="AO2" s="129"/>
-      <c r="AP2" s="127">
+      <c r="AN2" s="118"/>
+      <c r="AO2" s="119"/>
+      <c r="AP2" s="117">
         <v>13</v>
       </c>
-      <c r="AQ2" s="128"/>
-      <c r="AR2" s="129"/>
+      <c r="AQ2" s="118"/>
+      <c r="AR2" s="119"/>
     </row>
     <row r="3" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="130"/>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="120"/>
+      <c r="C3" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130" t="s">
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130" t="s">
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130" t="s">
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="130"/>
-      <c r="N3" s="130"/>
-      <c r="O3" s="130" t="s">
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="130"/>
-      <c r="Q3" s="130"/>
-      <c r="R3" s="130" t="s">
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="S3" s="130"/>
-      <c r="T3" s="130"/>
-      <c r="U3" s="130" t="s">
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="V3" s="130"/>
-      <c r="W3" s="130"/>
-      <c r="X3" s="130" t="s">
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="Y3" s="130"/>
-      <c r="Z3" s="130"/>
-      <c r="AA3" s="131" t="s">
+      <c r="Y3" s="120"/>
+      <c r="Z3" s="120"/>
+      <c r="AA3" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="AB3" s="132"/>
-      <c r="AC3" s="133"/>
-      <c r="AD3" s="130" t="s">
+      <c r="AB3" s="127"/>
+      <c r="AC3" s="128"/>
+      <c r="AD3" s="120" t="s">
         <v>30</v>
       </c>
-      <c r="AE3" s="130"/>
-      <c r="AF3" s="130"/>
-      <c r="AG3" s="130" t="s">
+      <c r="AE3" s="120"/>
+      <c r="AF3" s="120"/>
+      <c r="AG3" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="AH3" s="130"/>
-      <c r="AI3" s="130"/>
-      <c r="AJ3" s="130" t="s">
+      <c r="AH3" s="120"/>
+      <c r="AI3" s="120"/>
+      <c r="AJ3" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="AK3" s="130"/>
-      <c r="AL3" s="130"/>
-      <c r="AM3" s="130" t="s">
+      <c r="AK3" s="120"/>
+      <c r="AL3" s="120"/>
+      <c r="AM3" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="AN3" s="130"/>
-      <c r="AO3" s="130"/>
-      <c r="AP3" s="130" t="s">
+      <c r="AN3" s="120"/>
+      <c r="AO3" s="120"/>
+      <c r="AP3" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="130"/>
-      <c r="AR3" s="130"/>
+      <c r="AQ3" s="120"/>
+      <c r="AR3" s="120"/>
     </row>
     <row r="4" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="130" t="s">
+      <c r="A4" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="130"/>
+      <c r="B4" s="120"/>
       <c r="C4" s="14">
         <v>2006</v>
       </c>
@@ -20547,10 +20547,10 @@
       </c>
     </row>
     <row r="5" spans="1:44" s="14" customFormat="1" ht="20" customHeight="1">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="130"/>
+      <c r="B5" s="120"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -20679,7 +20679,7 @@
       </c>
     </row>
     <row r="6" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A6" s="139" t="s">
+      <c r="A6" s="125" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -20813,7 +20813,7 @@
       </c>
     </row>
     <row r="7" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="139"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="16" t="s">
         <v>34</v>
       </c>
@@ -20945,7 +20945,7 @@
       </c>
     </row>
     <row r="8" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="139"/>
+      <c r="A8" s="125"/>
       <c r="B8" s="16" t="s">
         <v>35</v>
       </c>
@@ -21077,7 +21077,7 @@
       </c>
     </row>
     <row r="9" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A9" s="139"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="15" t="s">
         <v>51</v>
       </c>
@@ -21209,7 +21209,7 @@
       </c>
     </row>
     <row r="10" spans="1:44" s="13" customFormat="1" ht="20" customHeight="1">
-      <c r="A10" s="139"/>
+      <c r="A10" s="125"/>
       <c r="B10" s="16" t="s">
         <v>36</v>
       </c>
@@ -21341,7 +21341,7 @@
       </c>
     </row>
     <row r="11" spans="1:44" ht="20" customHeight="1">
-      <c r="A11" s="134" t="s">
+      <c r="A11" s="121" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -21475,7 +21475,7 @@
       </c>
     </row>
     <row r="12" spans="1:44" ht="20" customHeight="1">
-      <c r="A12" s="134"/>
+      <c r="A12" s="121"/>
       <c r="B12" s="6" t="s">
         <v>39</v>
       </c>
@@ -21607,7 +21607,7 @@
       </c>
     </row>
     <row r="13" spans="1:44" ht="20" customHeight="1">
-      <c r="A13" s="134"/>
+      <c r="A13" s="121"/>
       <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
@@ -21739,7 +21739,7 @@
       </c>
     </row>
     <row r="14" spans="1:44" ht="20" customHeight="1">
-      <c r="A14" s="134"/>
+      <c r="A14" s="121"/>
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
@@ -21871,7 +21871,7 @@
       </c>
     </row>
     <row r="15" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="135" t="s">
+      <c r="A15" s="116" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -22005,7 +22005,7 @@
       </c>
     </row>
     <row r="16" spans="1:44" s="11" customFormat="1" ht="20" customHeight="1">
-      <c r="A16" s="135"/>
+      <c r="A16" s="116"/>
       <c r="B16" s="10" t="s">
         <v>43</v>
       </c>
@@ -22137,7 +22137,7 @@
       </c>
     </row>
     <row r="17" spans="1:44" ht="20" customHeight="1">
-      <c r="A17" s="134" t="s">
+      <c r="A17" s="121" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -22271,7 +22271,7 @@
       </c>
     </row>
     <row r="18" spans="1:44" ht="20" customHeight="1">
-      <c r="A18" s="134"/>
+      <c r="A18" s="121"/>
       <c r="B18" s="6" t="s">
         <v>46</v>
       </c>
@@ -22403,7 +22403,7 @@
       </c>
     </row>
     <row r="19" spans="1:44" ht="20" customHeight="1">
-      <c r="A19" s="134"/>
+      <c r="A19" s="121"/>
       <c r="B19" s="6" t="s">
         <v>47</v>
       </c>
@@ -23061,6 +23061,29 @@
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AM3:AO3"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="AG3:AI3"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="AA3:AC3"/>
     <mergeCell ref="AP2:AR2"/>
     <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="AJ2:AL2"/>
@@ -23074,29 +23097,6 @@
     <mergeCell ref="X2:Z2"/>
     <mergeCell ref="AD2:AF2"/>
     <mergeCell ref="AA2:AC2"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AP3:AR3"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="AG3:AI3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -23308,44 +23308,44 @@
     <row r="1" spans="1:19">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="139" t="s">
+      <c r="F1" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="139"/>
-      <c r="H1" s="139"/>
-      <c r="I1" s="139"/>
-      <c r="J1" s="139"/>
-      <c r="K1" s="134" t="s">
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="135" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="135"/>
-      <c r="Q1" s="134" t="s">
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="116" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="134"/>
-      <c r="S1" s="134"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
     </row>
     <row r="2" spans="1:19" ht="84">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
       <c r="F2" s="15" t="s">
         <v>0</v>
       </c>
@@ -23390,13 +23390,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="127">
-        <v>1</v>
-      </c>
-      <c r="C3" s="130" t="s">
+      <c r="B3" s="117">
+        <v>1</v>
+      </c>
+      <c r="C3" s="120" t="s">
         <v>50</v>
       </c>
       <c r="D3" s="14">
@@ -23449,9 +23449,9 @@
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="137"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="130"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="14">
         <v>2010</v>
       </c>
@@ -23502,9 +23502,9 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="137"/>
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
+      <c r="A5" s="123"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="120"/>
       <c r="D5" s="25">
         <v>2014</v>
       </c>
@@ -23555,11 +23555,11 @@
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="137"/>
-      <c r="B6" s="127">
+      <c r="A6" s="123"/>
+      <c r="B6" s="117">
         <v>2</v>
       </c>
-      <c r="C6" s="130" t="s">
+      <c r="C6" s="120" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="14">
@@ -23612,9 +23612,9 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="137"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="130"/>
+      <c r="A7" s="123"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="120"/>
       <c r="D7" s="14">
         <v>2010</v>
       </c>
@@ -23665,9 +23665,9 @@
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="137"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="130"/>
+      <c r="A8" s="123"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="120"/>
       <c r="D8" s="25">
         <v>2014</v>
       </c>
@@ -23718,11 +23718,11 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="137"/>
-      <c r="B9" s="127">
+      <c r="A9" s="123"/>
+      <c r="B9" s="117">
         <v>3</v>
       </c>
-      <c r="C9" s="130" t="s">
+      <c r="C9" s="120" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="14">
@@ -23775,9 +23775,9 @@
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="137"/>
-      <c r="B10" s="128"/>
-      <c r="C10" s="130"/>
+      <c r="A10" s="123"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="120"/>
       <c r="D10" s="14">
         <v>2010</v>
       </c>
@@ -23828,9 +23828,9 @@
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="137"/>
-      <c r="B11" s="129"/>
-      <c r="C11" s="130"/>
+      <c r="A11" s="123"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="120"/>
       <c r="D11" s="25">
         <v>2014</v>
       </c>
@@ -23881,11 +23881,11 @@
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="137"/>
-      <c r="B12" s="127">
+      <c r="A12" s="123"/>
+      <c r="B12" s="117">
         <v>4</v>
       </c>
-      <c r="C12" s="130" t="s">
+      <c r="C12" s="120" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="14">
@@ -23938,9 +23938,9 @@
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="137"/>
-      <c r="B13" s="128"/>
-      <c r="C13" s="130"/>
+      <c r="A13" s="123"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="120"/>
       <c r="D13" s="14">
         <v>2010</v>
       </c>
@@ -23991,9 +23991,9 @@
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="137"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="130"/>
+      <c r="A14" s="123"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="120"/>
       <c r="D14" s="25">
         <v>2014</v>
       </c>
@@ -24044,11 +24044,11 @@
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="137"/>
-      <c r="B15" s="127">
+      <c r="A15" s="123"/>
+      <c r="B15" s="117">
         <v>5</v>
       </c>
-      <c r="C15" s="130" t="s">
+      <c r="C15" s="120" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="14">
@@ -24101,9 +24101,9 @@
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="137"/>
-      <c r="B16" s="128"/>
-      <c r="C16" s="130"/>
+      <c r="A16" s="123"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="120"/>
       <c r="D16" s="14">
         <v>2010</v>
       </c>
@@ -24154,9 +24154,9 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="137"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="130"/>
+      <c r="A17" s="123"/>
+      <c r="B17" s="119"/>
+      <c r="C17" s="120"/>
       <c r="D17" s="25">
         <v>2014</v>
       </c>
@@ -24207,11 +24207,11 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="137"/>
-      <c r="B18" s="127">
+      <c r="A18" s="123"/>
+      <c r="B18" s="117">
         <v>6</v>
       </c>
-      <c r="C18" s="130" t="s">
+      <c r="C18" s="120" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="14">
@@ -24264,9 +24264,9 @@
       </c>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="137"/>
-      <c r="B19" s="128"/>
-      <c r="C19" s="130"/>
+      <c r="A19" s="123"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="120"/>
       <c r="D19" s="14">
         <v>2010</v>
       </c>
@@ -24317,9 +24317,9 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="137"/>
-      <c r="B20" s="129"/>
-      <c r="C20" s="130"/>
+      <c r="A20" s="123"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="120"/>
       <c r="D20" s="25">
         <v>2014</v>
       </c>
@@ -24370,11 +24370,11 @@
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="137"/>
-      <c r="B21" s="127">
+      <c r="A21" s="123"/>
+      <c r="B21" s="117">
         <v>7</v>
       </c>
-      <c r="C21" s="130" t="s">
+      <c r="C21" s="120" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="14">
@@ -24427,9 +24427,9 @@
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="137"/>
-      <c r="B22" s="128"/>
-      <c r="C22" s="130"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="120"/>
       <c r="D22" s="14">
         <v>2010</v>
       </c>
@@ -24480,9 +24480,9 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="137"/>
-      <c r="B23" s="129"/>
-      <c r="C23" s="130"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="120"/>
       <c r="D23" s="25">
         <v>2014</v>
       </c>
@@ -24533,11 +24533,11 @@
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="137"/>
-      <c r="B24" s="127">
+      <c r="A24" s="123"/>
+      <c r="B24" s="117">
         <v>8</v>
       </c>
-      <c r="C24" s="130" t="s">
+      <c r="C24" s="120" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="14">
@@ -24590,9 +24590,9 @@
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="137"/>
-      <c r="B25" s="128"/>
-      <c r="C25" s="130"/>
+      <c r="A25" s="123"/>
+      <c r="B25" s="118"/>
+      <c r="C25" s="120"/>
       <c r="D25" s="14">
         <v>2010</v>
       </c>
@@ -24643,9 +24643,9 @@
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="137"/>
-      <c r="B26" s="129"/>
-      <c r="C26" s="130"/>
+      <c r="A26" s="123"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="120"/>
       <c r="D26" s="25">
         <v>2014</v>
       </c>
@@ -24696,11 +24696,11 @@
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="137"/>
-      <c r="B27" s="127">
+      <c r="A27" s="123"/>
+      <c r="B27" s="117">
         <v>14</v>
       </c>
-      <c r="C27" s="131" t="s">
+      <c r="C27" s="126" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="14">
@@ -24753,9 +24753,9 @@
       </c>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="137"/>
-      <c r="B28" s="128"/>
-      <c r="C28" s="132"/>
+      <c r="A28" s="123"/>
+      <c r="B28" s="118"/>
+      <c r="C28" s="127"/>
       <c r="D28" s="14">
         <v>2010</v>
       </c>
@@ -24806,9 +24806,9 @@
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="137"/>
-      <c r="B29" s="129"/>
-      <c r="C29" s="133"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="128"/>
       <c r="D29" s="25">
         <v>2014</v>
       </c>
@@ -24859,11 +24859,11 @@
       </c>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="137"/>
-      <c r="B30" s="127">
+      <c r="A30" s="123"/>
+      <c r="B30" s="117">
         <v>9</v>
       </c>
-      <c r="C30" s="130" t="s">
+      <c r="C30" s="120" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="14">
@@ -24916,9 +24916,9 @@
       </c>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="137"/>
-      <c r="B31" s="128"/>
-      <c r="C31" s="130"/>
+      <c r="A31" s="123"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="120"/>
       <c r="D31" s="14">
         <v>2010</v>
       </c>
@@ -24969,9 +24969,9 @@
       </c>
     </row>
     <row r="32" spans="1:19">
-      <c r="A32" s="137"/>
-      <c r="B32" s="129"/>
-      <c r="C32" s="130"/>
+      <c r="A32" s="123"/>
+      <c r="B32" s="119"/>
+      <c r="C32" s="120"/>
       <c r="D32" s="25">
         <v>2014</v>
       </c>
@@ -25022,11 +25022,11 @@
       </c>
     </row>
     <row r="33" spans="1:41">
-      <c r="A33" s="137"/>
-      <c r="B33" s="127">
+      <c r="A33" s="123"/>
+      <c r="B33" s="117">
         <v>10</v>
       </c>
-      <c r="C33" s="130" t="s">
+      <c r="C33" s="120" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="14">
@@ -25079,9 +25079,9 @@
       </c>
     </row>
     <row r="34" spans="1:41">
-      <c r="A34" s="137"/>
-      <c r="B34" s="128"/>
-      <c r="C34" s="130"/>
+      <c r="A34" s="123"/>
+      <c r="B34" s="118"/>
+      <c r="C34" s="120"/>
       <c r="D34" s="14">
         <v>2010</v>
       </c>
@@ -25132,9 +25132,9 @@
       </c>
     </row>
     <row r="35" spans="1:41">
-      <c r="A35" s="137"/>
-      <c r="B35" s="129"/>
-      <c r="C35" s="130"/>
+      <c r="A35" s="123"/>
+      <c r="B35" s="119"/>
+      <c r="C35" s="120"/>
       <c r="D35" s="25">
         <v>2014</v>
       </c>
@@ -25185,11 +25185,11 @@
       </c>
     </row>
     <row r="36" spans="1:41">
-      <c r="A36" s="137"/>
-      <c r="B36" s="127">
+      <c r="A36" s="123"/>
+      <c r="B36" s="117">
         <v>11</v>
       </c>
-      <c r="C36" s="130" t="s">
+      <c r="C36" s="120" t="s">
         <v>21</v>
       </c>
       <c r="D36" s="14">
@@ -25242,9 +25242,9 @@
       </c>
     </row>
     <row r="37" spans="1:41">
-      <c r="A37" s="137"/>
-      <c r="B37" s="128"/>
-      <c r="C37" s="130"/>
+      <c r="A37" s="123"/>
+      <c r="B37" s="118"/>
+      <c r="C37" s="120"/>
       <c r="D37" s="14">
         <v>2010</v>
       </c>
@@ -25295,9 +25295,9 @@
       </c>
     </row>
     <row r="38" spans="1:41">
-      <c r="A38" s="137"/>
-      <c r="B38" s="129"/>
-      <c r="C38" s="130"/>
+      <c r="A38" s="123"/>
+      <c r="B38" s="119"/>
+      <c r="C38" s="120"/>
       <c r="D38" s="25">
         <v>2014</v>
       </c>
@@ -25348,11 +25348,11 @@
       </c>
     </row>
     <row r="39" spans="1:41">
-      <c r="A39" s="137"/>
-      <c r="B39" s="127">
+      <c r="A39" s="123"/>
+      <c r="B39" s="117">
         <v>12</v>
       </c>
-      <c r="C39" s="130" t="s">
+      <c r="C39" s="120" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="14">
@@ -25405,9 +25405,9 @@
       </c>
     </row>
     <row r="40" spans="1:41">
-      <c r="A40" s="137"/>
-      <c r="B40" s="128"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="123"/>
+      <c r="B40" s="118"/>
+      <c r="C40" s="120"/>
       <c r="D40" s="14">
         <v>2010</v>
       </c>
@@ -25458,9 +25458,9 @@
       </c>
     </row>
     <row r="41" spans="1:41">
-      <c r="A41" s="137"/>
-      <c r="B41" s="129"/>
-      <c r="C41" s="130"/>
+      <c r="A41" s="123"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="120"/>
       <c r="D41" s="25">
         <v>2014</v>
       </c>
@@ -25511,11 +25511,11 @@
       </c>
     </row>
     <row r="42" spans="1:41">
-      <c r="A42" s="137"/>
-      <c r="B42" s="127">
+      <c r="A42" s="123"/>
+      <c r="B42" s="117">
         <v>13</v>
       </c>
-      <c r="C42" s="130" t="s">
+      <c r="C42" s="120" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="14">
@@ -25568,9 +25568,9 @@
       </c>
     </row>
     <row r="43" spans="1:41">
-      <c r="A43" s="137"/>
-      <c r="B43" s="128"/>
-      <c r="C43" s="130"/>
+      <c r="A43" s="123"/>
+      <c r="B43" s="118"/>
+      <c r="C43" s="120"/>
       <c r="D43" s="14">
         <v>2010</v>
       </c>
@@ -25621,9 +25621,9 @@
       </c>
     </row>
     <row r="44" spans="1:41">
-      <c r="A44" s="138"/>
-      <c r="B44" s="129"/>
-      <c r="C44" s="130"/>
+      <c r="A44" s="124"/>
+      <c r="B44" s="119"/>
+      <c r="C44" s="120"/>
       <c r="D44" s="25">
         <v>2014</v>
       </c>
@@ -25674,81 +25674,81 @@
       </c>
     </row>
     <row r="46" spans="1:41" ht="15.75" customHeight="1">
-      <c r="A46" s="130" t="s">
+      <c r="A46" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="130"/>
-      <c r="C46" s="130" t="s">
+      <c r="B46" s="120"/>
+      <c r="C46" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="D46" s="130"/>
-      <c r="E46" s="130"/>
-      <c r="F46" s="130" t="s">
+      <c r="D46" s="120"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="130"/>
-      <c r="H46" s="130"/>
-      <c r="I46" s="130" t="s">
+      <c r="G46" s="120"/>
+      <c r="H46" s="120"/>
+      <c r="I46" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="J46" s="130"/>
-      <c r="K46" s="130"/>
-      <c r="L46" s="130" t="s">
+      <c r="J46" s="120"/>
+      <c r="K46" s="120"/>
+      <c r="L46" s="120" t="s">
         <v>10</v>
       </c>
-      <c r="M46" s="130"/>
-      <c r="N46" s="130"/>
-      <c r="O46" s="130" t="s">
+      <c r="M46" s="120"/>
+      <c r="N46" s="120"/>
+      <c r="O46" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="P46" s="130"/>
-      <c r="Q46" s="130"/>
-      <c r="R46" s="130" t="s">
+      <c r="P46" s="120"/>
+      <c r="Q46" s="120"/>
+      <c r="R46" s="120" t="s">
         <v>87</v>
       </c>
-      <c r="S46" s="130"/>
-      <c r="T46" s="130"/>
-      <c r="U46" s="131" t="s">
+      <c r="S46" s="120"/>
+      <c r="T46" s="120"/>
+      <c r="U46" s="126" t="s">
         <v>70</v>
       </c>
-      <c r="V46" s="132"/>
-      <c r="W46" s="133"/>
-      <c r="X46" s="131" t="s">
+      <c r="V46" s="127"/>
+      <c r="W46" s="128"/>
+      <c r="X46" s="126" t="s">
         <v>54</v>
       </c>
-      <c r="Y46" s="132"/>
-      <c r="Z46" s="133"/>
-      <c r="AA46" s="130" t="s">
+      <c r="Y46" s="127"/>
+      <c r="Z46" s="128"/>
+      <c r="AA46" s="120" t="s">
         <v>12</v>
       </c>
-      <c r="AB46" s="130"/>
-      <c r="AC46" s="130"/>
-      <c r="AD46" s="130" t="s">
+      <c r="AB46" s="120"/>
+      <c r="AC46" s="120"/>
+      <c r="AD46" s="120" t="s">
         <v>28</v>
       </c>
-      <c r="AE46" s="130"/>
-      <c r="AF46" s="130"/>
-      <c r="AG46" s="130" t="s">
+      <c r="AE46" s="120"/>
+      <c r="AF46" s="120"/>
+      <c r="AG46" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="AH46" s="130"/>
-      <c r="AI46" s="130"/>
-      <c r="AJ46" s="130" t="s">
+      <c r="AH46" s="120"/>
+      <c r="AI46" s="120"/>
+      <c r="AJ46" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="AK46" s="130"/>
-      <c r="AL46" s="130"/>
-      <c r="AM46" s="130" t="s">
+      <c r="AK46" s="120"/>
+      <c r="AL46" s="120"/>
+      <c r="AM46" s="120" t="s">
         <v>8</v>
       </c>
-      <c r="AN46" s="130"/>
-      <c r="AO46" s="130"/>
+      <c r="AN46" s="120"/>
+      <c r="AO46" s="120"/>
     </row>
     <row r="47" spans="1:41" ht="42.75" customHeight="1">
-      <c r="A47" s="130" t="s">
+      <c r="A47" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="130"/>
+      <c r="B47" s="120"/>
       <c r="C47" s="54" t="s">
         <v>72</v>
       </c>
@@ -25868,10 +25868,10 @@
       </c>
     </row>
     <row r="48" spans="1:41" ht="33" customHeight="1">
-      <c r="A48" s="130" t="s">
+      <c r="A48" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="130"/>
+      <c r="B48" s="120"/>
       <c r="C48" s="54">
         <v>4</v>
       </c>
@@ -25991,7 +25991,7 @@
       </c>
     </row>
     <row r="49" spans="2:4">
-      <c r="B49" s="141" t="s">
+      <c r="B49" s="143" t="s">
         <v>91</v>
       </c>
       <c r="C49" s="63">
@@ -26002,7 +26002,7 @@
       </c>
     </row>
     <row r="50" spans="2:4">
-      <c r="B50" s="120"/>
+      <c r="B50" s="136"/>
       <c r="C50" s="63">
         <v>2010</v>
       </c>
@@ -26011,7 +26011,7 @@
       </c>
     </row>
     <row r="51" spans="2:4">
-      <c r="B51" s="120"/>
+      <c r="B51" s="136"/>
       <c r="C51" s="63">
         <v>2014</v>
       </c>
@@ -26021,23 +26021,26 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="AA46:AC46"/>
-    <mergeCell ref="AD46:AF46"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="AG46:AI46"/>
-    <mergeCell ref="AJ46:AL46"/>
-    <mergeCell ref="AM46:AO46"/>
-    <mergeCell ref="O46:Q46"/>
-    <mergeCell ref="R46:T46"/>
-    <mergeCell ref="U46:W46"/>
-    <mergeCell ref="X46:Z46"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="B42:B44"/>
@@ -26054,26 +26057,23 @@
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="AG46:AI46"/>
+    <mergeCell ref="AJ46:AL46"/>
+    <mergeCell ref="AM46:AO46"/>
+    <mergeCell ref="O46:Q46"/>
+    <mergeCell ref="R46:T46"/>
+    <mergeCell ref="U46:W46"/>
+    <mergeCell ref="X46:Z46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="AA46:AC46"/>
+    <mergeCell ref="AD46:AF46"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="L46:N46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>